<commit_message>
se agrego la Clase de Equivalencia para Categoria
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M1.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2b6b49da01230f2/Documentos/proyecto wong/Softgenix-Peru/2-Desarrollo/SCIP/pruebas-calidad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_8AF91C39AE0E0FE7D0B96C6DE05857BA94B61638" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B45971E-3504-4220-BDD9-62C462B3FA29}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="11_8AF91C39AE0E0FE7D0B96C6DE05857BA94B61638" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26DDD037-B5A7-4F89-A351-32D818C25EF1}"/>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="1890" windowWidth="17925" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7320" yWindow="3630" windowWidth="17925" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clase equivalencia categoria" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -116,13 +116,52 @@
   </si>
   <si>
     <t>CP12</t>
+  </si>
+  <si>
+    <t>Identificador</t>
+  </si>
+  <si>
+    <t>Logico</t>
+  </si>
+  <si>
+    <t>ID= caracteres alfanumericos</t>
+  </si>
+  <si>
+    <t>CEV&lt;1&gt;</t>
+  </si>
+  <si>
+    <t>ID !=caracteres alfanumericos</t>
+  </si>
+  <si>
+    <t>CENV&lt;01&gt;</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>1&lt;ID&lt;=32</t>
+  </si>
+  <si>
+    <t>CEV&lt;2&gt;</t>
+  </si>
+  <si>
+    <t>ID&lt;1</t>
+  </si>
+  <si>
+    <t>CENV&lt;02&gt;</t>
+  </si>
+  <si>
+    <t>ID&gt;32</t>
+  </si>
+  <si>
+    <t>CENV&lt;03&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -150,11 +189,6 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -179,6 +213,30 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Garamond"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -237,7 +295,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -281,55 +339,9 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -343,40 +355,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -386,117 +386,132 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,16 +533,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>30595</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>116320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -556,7 +571,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8162925" y="1238250"/>
+          <a:off x="1647825" y="3429000"/>
           <a:ext cx="7772400" cy="4278745"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -567,6 +582,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -770,7 +789,7 @@
   <dimension ref="B1:P1002"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -779,336 +798,315 @@
     <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="4" max="4" width="24.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" customWidth="1"/>
-    <col min="7" max="26" width="10" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" customWidth="1"/>
+    <col min="9" max="26" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="41" t="s">
+    <row r="1" spans="3:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="3:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="44"/>
+      <c r="G3" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="42"/>
-    </row>
-    <row r="4" spans="2:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
+      <c r="H3" s="44"/>
+    </row>
+    <row r="4" spans="3:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="45" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="43"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="2:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="44"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="2:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="45"/>
+    <row r="5" spans="3:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="48" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="44"/>
+      <c r="D6" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="48" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="44"/>
       <c r="D7" s="44"/>
       <c r="E7" s="44"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="43"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="2:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="44"/>
-      <c r="C9" s="43"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="48" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="46"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+    </row>
+    <row r="9" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="44"/>
       <c r="D9" s="46"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="2:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="45"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+    </row>
+    <row r="10" spans="3:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="44"/>
       <c r="D10" s="44"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="43"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="45"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="48"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="46"/>
-    </row>
-    <row r="14" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="44"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-    </row>
-    <row r="15" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="45"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-    </row>
-    <row r="16" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="43"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-    </row>
-    <row r="17" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-    </row>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+    </row>
+    <row r="11" spans="3:8" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="3:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="3:8" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="3:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="3:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="3:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="44"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="7"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
     </row>
     <row r="19" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
     </row>
     <row r="20" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="21" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I22" s="10"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="49"/>
-      <c r="M22" s="50"/>
-      <c r="N22" s="49"/>
-      <c r="O22" s="50"/>
-      <c r="P22" s="10"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="33"/>
+      <c r="N22" s="34"/>
+      <c r="O22" s="33"/>
+      <c r="P22" s="1"/>
     </row>
     <row r="23" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="11"/>
-      <c r="O23" s="12"/>
-      <c r="P23" s="10"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="1"/>
     </row>
     <row r="24" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="11"/>
-      <c r="O24" s="51"/>
-      <c r="P24" s="10"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="32"/>
+      <c r="P24" s="1"/>
     </row>
     <row r="25" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11"/>
-      <c r="O25" s="50"/>
-      <c r="P25" s="10"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="33"/>
+      <c r="P25" s="1"/>
     </row>
     <row r="26" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
-      <c r="M26" s="11"/>
-      <c r="N26" s="11"/>
-      <c r="O26" s="51"/>
-      <c r="P26" s="10"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="32"/>
+      <c r="P26" s="1"/>
     </row>
     <row r="27" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
-      <c r="N27" s="11"/>
-      <c r="O27" s="50"/>
-      <c r="P27" s="10"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="33"/>
+      <c r="P27" s="1"/>
     </row>
     <row r="28" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
-      <c r="M28" s="11"/>
-      <c r="N28" s="11"/>
-      <c r="O28" s="51"/>
-      <c r="P28" s="10"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="32"/>
+      <c r="P28" s="1"/>
     </row>
     <row r="29" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
-      <c r="L29" s="11"/>
-      <c r="M29" s="11"/>
-      <c r="N29" s="11"/>
-      <c r="O29" s="50"/>
-      <c r="P29" s="10"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="33"/>
+      <c r="P29" s="1"/>
     </row>
     <row r="30" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="11"/>
-      <c r="N30" s="11"/>
-      <c r="O30" s="13"/>
-      <c r="P30" s="10"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="1"/>
     </row>
     <row r="31" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="11"/>
-      <c r="M31" s="11"/>
-      <c r="N31" s="11"/>
-      <c r="O31" s="13"/>
-      <c r="P31" s="10"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="1"/>
     </row>
     <row r="32" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-      <c r="L32" s="11"/>
-      <c r="M32" s="11"/>
-      <c r="N32" s="11"/>
-      <c r="O32" s="13"/>
-      <c r="P32" s="10"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="1"/>
     </row>
     <row r="33" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
-      <c r="N33" s="11"/>
-      <c r="O33" s="13"/>
-      <c r="P33" s="10"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="1"/>
     </row>
     <row r="34" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="11"/>
-      <c r="M34" s="11"/>
-      <c r="N34" s="11"/>
-      <c r="O34" s="13"/>
-      <c r="P34" s="10"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="1"/>
     </row>
     <row r="35" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I35" s="11"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="11"/>
-      <c r="L35" s="11"/>
-      <c r="M35" s="11"/>
-      <c r="N35" s="11"/>
-      <c r="O35" s="13"/>
-      <c r="P35" s="10"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="1"/>
     </row>
     <row r="36" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="11"/>
-      <c r="L36" s="11"/>
-      <c r="M36" s="11"/>
-      <c r="N36" s="11"/>
-      <c r="O36" s="13"/>
-      <c r="P36" s="10"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="1"/>
     </row>
     <row r="37" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="11"/>
-      <c r="L37" s="11"/>
-      <c r="M37" s="11"/>
-      <c r="N37" s="11"/>
-      <c r="O37" s="10"/>
-      <c r="P37" s="10"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
     </row>
     <row r="38" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="11"/>
-      <c r="L38" s="11"/>
-      <c r="M38" s="11"/>
-      <c r="N38" s="11"/>
-      <c r="O38" s="10"/>
-      <c r="P38" s="10"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
     </row>
     <row r="39" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="40" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2075,33 +2073,22 @@
     <row r="1001" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="15">
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="N22:O22"/>
     <mergeCell ref="O24:O25"/>
     <mergeCell ref="O26:O27"/>
     <mergeCell ref="O28:O29"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G16:G17"/>
     <mergeCell ref="L22:M22"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="F13:F15"/>
-    <mergeCell ref="G13:G15"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -2131,243 +2118,243 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="42"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="35"/>
     </row>
     <row r="3" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="53" t="s">
+      <c r="J3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="54"/>
-      <c r="L3" s="42"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="35"/>
     </row>
     <row r="4" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
     </row>
     <row r="5" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
     </row>
     <row r="6" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
     </row>
     <row r="7" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
     </row>
     <row r="8" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
     </row>
     <row r="9" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
     </row>
     <row r="10" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
     </row>
     <row r="11" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
     </row>
     <row r="12" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
     </row>
     <row r="13" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
     </row>
     <row r="14" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="34"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
     </row>
     <row r="15" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="38"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="29"/>
     </row>
     <row r="16" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
se actualizo la Clase de Equivalencia para Categoria
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M1.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2b6b49da01230f2/Documentos/proyecto wong/Softgenix-Peru/2-Desarrollo/SCIP/pruebas-calidad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="11_8AF91C39AE0E0FE7D0B96C6DE05857BA94B61638" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26DDD037-B5A7-4F89-A351-32D818C25EF1}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="11_8AF91C39AE0E0FE7D0B96C6DE05857BA94B61638" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{086CA80D-76B0-4818-9E56-695A19C2019E}"/>
   <bookViews>
     <workbookView xWindow="7320" yWindow="3630" windowWidth="17925" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -155,6 +155,33 @@
   </si>
   <si>
     <t>CENV&lt;03&gt;</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>descripcion= caracteres alfanumericos</t>
+  </si>
+  <si>
+    <t>descripcion != caracteres alfanumericos</t>
+  </si>
+  <si>
+    <t>CENV&lt;04&gt;</t>
+  </si>
+  <si>
+    <t>0&lt;=ID&lt;=50</t>
+  </si>
+  <si>
+    <t>descripcion&lt;1</t>
+  </si>
+  <si>
+    <t>CENV&lt;05&gt;</t>
+  </si>
+  <si>
+    <t>descripcion&gt;50</t>
+  </si>
+  <si>
+    <t>CENV&lt;06&gt;</t>
   </si>
 </sst>
 </file>
@@ -374,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -467,51 +494,50 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -789,7 +815,7 @@
   <dimension ref="B1:P1002"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -808,110 +834,136 @@
     <row r="1" spans="3:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="3:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="43" t="s">
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="44"/>
-      <c r="G3" s="43" t="s">
+      <c r="F3" s="39"/>
+      <c r="G3" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="44"/>
+      <c r="H3" s="39"/>
     </row>
     <row r="4" spans="3:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="45" t="s">
+      <c r="F4" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="45" t="s">
+      <c r="G4" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="45" t="s">
+      <c r="H4" s="35" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="3:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="48" t="s">
+      <c r="G5" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="48" t="s">
+      <c r="H5" s="37" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="3:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="44"/>
-      <c r="D6" s="46" t="s">
+      <c r="C6" s="39"/>
+      <c r="D6" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="49" t="s">
+      <c r="E6" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="49" t="s">
+      <c r="F6" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="48" t="s">
+      <c r="G6" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="48" t="s">
+      <c r="H6" s="37" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="7" spans="3:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="48" t="s">
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="48" t="s">
+      <c r="H7" s="37" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="8" spans="3:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="46"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
+      <c r="C8" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="37" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="9" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="44"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="37" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="10" spans="3:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="48"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="37" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="11" spans="3:8" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="3:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -920,21 +972,14 @@
     <row r="15" spans="3:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="16" spans="3:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-    </row>
+    <row r="18" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
     </row>
     <row r="20" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="21" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -942,10 +987,10 @@
       <c r="I22" s="1"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
-      <c r="L22" s="34"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="34"/>
-      <c r="O22" s="33"/>
+      <c r="L22" s="43"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="43"/>
+      <c r="O22" s="44"/>
       <c r="P22" s="1"/>
     </row>
     <row r="23" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -965,7 +1010,7 @@
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
-      <c r="O24" s="32"/>
+      <c r="O24" s="45"/>
       <c r="P24" s="1"/>
     </row>
     <row r="25" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -975,7 +1020,7 @@
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
-      <c r="O25" s="33"/>
+      <c r="O25" s="44"/>
       <c r="P25" s="1"/>
     </row>
     <row r="26" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -985,7 +1030,7 @@
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
-      <c r="O26" s="32"/>
+      <c r="O26" s="45"/>
       <c r="P26" s="1"/>
     </row>
     <row r="27" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -995,7 +1040,7 @@
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
-      <c r="O27" s="33"/>
+      <c r="O27" s="44"/>
       <c r="P27" s="1"/>
     </row>
     <row r="28" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1005,7 +1050,7 @@
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
-      <c r="O28" s="32"/>
+      <c r="O28" s="45"/>
       <c r="P28" s="1"/>
     </row>
     <row r="29" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1015,7 +1060,7 @@
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
-      <c r="O29" s="33"/>
+      <c r="O29" s="44"/>
       <c r="P29" s="1"/>
     </row>
     <row r="30" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2074,21 +2119,21 @@
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="O26:O27"/>
+    <mergeCell ref="O28:O29"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="C8:C10"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="O26:O27"/>
-    <mergeCell ref="O28:O29"/>
-    <mergeCell ref="L22:M22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -2118,20 +2163,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="35"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="49"/>
     </row>
     <row r="3" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -2161,11 +2206,11 @@
       <c r="I3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="37" t="s">
+      <c r="J3" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="38"/>
-      <c r="L3" s="35"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="49"/>
     </row>
     <row r="4" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">

</xml_diff>

<commit_message>
Se actualizo el documento de pruebas CE Agregar Categoria
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M1.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2b6b49da01230f2/Documentos/proyecto wong/Softgenix-Peru/2-Desarrollo/SCIP/pruebas-calidad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="11_8AF91C39AE0E0FE7D0B96C6DE05857BA94B61638" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{086CA80D-76B0-4818-9E56-695A19C2019E}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="11_8AF91C39AE0E0FE7D0B96C6DE05857BA94B61638" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8698F2D4-E9EC-441A-9427-513FEC1186EC}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="3630" windowWidth="17925" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="7320" yWindow="3630" windowWidth="17925" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clase equivalencia categoria" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -127,9 +127,6 @@
     <t>ID= caracteres alfanumericos</t>
   </si>
   <si>
-    <t>CEV&lt;1&gt;</t>
-  </si>
-  <si>
     <t>ID !=caracteres alfanumericos</t>
   </si>
   <si>
@@ -142,9 +139,6 @@
     <t>1&lt;ID&lt;=32</t>
   </si>
   <si>
-    <t>CEV&lt;2&gt;</t>
-  </si>
-  <si>
     <t>ID&lt;1</t>
   </si>
   <si>
@@ -160,12 +154,6 @@
     <t>Descripcion</t>
   </si>
   <si>
-    <t>descripcion= caracteres alfanumericos</t>
-  </si>
-  <si>
-    <t>descripcion != caracteres alfanumericos</t>
-  </si>
-  <si>
     <t>CENV&lt;04&gt;</t>
   </si>
   <si>
@@ -182,13 +170,37 @@
   </si>
   <si>
     <t>CENV&lt;06&gt;</t>
+  </si>
+  <si>
+    <t>CEV&lt;01&gt;</t>
+  </si>
+  <si>
+    <t>CEV&lt;02&gt;</t>
+  </si>
+  <si>
+    <t>ID=NULL</t>
+  </si>
+  <si>
+    <t>CEV&lt;03&gt;</t>
+  </si>
+  <si>
+    <t>descripcion= caracteres alfabetico</t>
+  </si>
+  <si>
+    <t>CEV&lt;04&gt;</t>
+  </si>
+  <si>
+    <t>descripcion != caracteres alfabetico</t>
+  </si>
+  <si>
+    <t>CEV&lt;05&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -196,56 +208,53 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Garamond"/>
-      <family val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -264,6 +273,13 @@
       <color rgb="FF000000"/>
       <name val="Garamond"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -322,7 +338,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -397,150 +413,185 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{4FE11987-A7A7-4235-AF2D-82033F1DCB3F}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -560,15 +611,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>116320</xdr:rowOff>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>30595</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -597,7 +648,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1647825" y="3429000"/>
+          <a:off x="1762125" y="2857500"/>
           <a:ext cx="7772400" cy="4278745"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -812,10 +863,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:P1002"/>
+  <dimension ref="B1:P994"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -831,338 +882,352 @@
     <col min="9" max="26" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="3:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="42" t="s">
+    <row r="1" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="2:16" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="2:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="39"/>
-      <c r="G3" s="42" t="s">
+      <c r="F5" s="36"/>
+      <c r="G5" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="39"/>
-    </row>
-    <row r="4" spans="3:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="35" t="s">
+      <c r="H5" s="36"/>
+    </row>
+    <row r="6" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D6" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E6" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="F6" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G6" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="35" t="s">
+      <c r="H6" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="3:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="40" t="s">
+    <row r="7" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D7" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E7" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="F7" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="37" t="s">
+      <c r="H7" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="37" t="s">
+    </row>
+    <row r="8" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="41"/>
+      <c r="D8" s="38" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="3:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="39"/>
-      <c r="D6" s="40" t="s">
+      <c r="E8" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="41" t="s">
+      <c r="F8" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="41" t="s">
+      <c r="H8" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="37" t="s">
+    </row>
+    <row r="9" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="37" t="s">
+      <c r="H9" s="40" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="3:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="37" t="s">
+    <row r="10" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+    </row>
+    <row r="11" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="28"/>
+      <c r="C11" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="37" t="s">
+      <c r="D11" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" s="40" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="3:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="40" t="s">
+    <row r="12" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C12" s="36"/>
+      <c r="D12" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="37" t="s">
+      <c r="F12" s="46" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="37" t="s">
+      <c r="H12" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="H8" s="37" t="s">
+    </row>
+    <row r="13" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="40" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="9" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="39"/>
-      <c r="D9" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="41" t="s">
+      <c r="H13" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" s="37" t="s">
-        <v>48</v>
-      </c>
-      <c r="H9" s="37" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="3:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="H10" s="37" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="3:8" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="3:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="3:8" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="3:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="3:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="3:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-    </row>
-    <row r="20" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I22" s="1"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="43"/>
-      <c r="M22" s="44"/>
-      <c r="N22" s="43"/>
-      <c r="O22" s="44"/>
-      <c r="P22" s="1"/>
-    </row>
-    <row r="23" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="1"/>
-    </row>
-    <row r="24" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="45"/>
-      <c r="P24" s="1"/>
-    </row>
-    <row r="25" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="44"/>
-      <c r="P25" s="1"/>
-    </row>
-    <row r="26" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="45"/>
-      <c r="P26" s="1"/>
-    </row>
-    <row r="27" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="44"/>
-      <c r="P27" s="1"/>
-    </row>
-    <row r="28" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="45"/>
-      <c r="P28" s="1"/>
-    </row>
-    <row r="29" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="44"/>
-      <c r="P29" s="1"/>
-    </row>
-    <row r="30" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="4"/>
-      <c r="P30" s="1"/>
-    </row>
-    <row r="31" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="1"/>
-    </row>
-    <row r="32" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="1"/>
-    </row>
-    <row r="33" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="1"/>
-    </row>
-    <row r="34" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-      <c r="O34" s="4"/>
-      <c r="P34" s="1"/>
-    </row>
-    <row r="35" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="1"/>
-    </row>
-    <row r="36" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="1"/>
-    </row>
-    <row r="37" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
-      <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
-    </row>
-    <row r="38" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
-    </row>
-    <row r="39" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="14" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I14" s="47"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="47"/>
+      <c r="N14" s="47"/>
+      <c r="O14" s="47"/>
+      <c r="P14" s="47"/>
+    </row>
+    <row r="15" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I15" s="47"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="47"/>
+      <c r="O15" s="47"/>
+      <c r="P15" s="47"/>
+    </row>
+    <row r="16" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="47"/>
+      <c r="O16" s="47"/>
+      <c r="P16" s="47"/>
+    </row>
+    <row r="17" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="47"/>
+      <c r="O17" s="47"/>
+      <c r="P17" s="47"/>
+    </row>
+    <row r="18" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="47"/>
+      <c r="L18" s="47"/>
+      <c r="M18" s="47"/>
+      <c r="N18" s="47"/>
+      <c r="O18" s="47"/>
+      <c r="P18" s="47"/>
+    </row>
+    <row r="19" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
+      <c r="K19" s="47"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="47"/>
+      <c r="N19" s="47"/>
+      <c r="O19" s="47"/>
+      <c r="P19" s="47"/>
+    </row>
+    <row r="20" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I20" s="47"/>
+      <c r="J20" s="47"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="47"/>
+      <c r="M20" s="47"/>
+      <c r="N20" s="47"/>
+      <c r="O20" s="47"/>
+      <c r="P20" s="47"/>
+    </row>
+    <row r="21" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I21" s="47"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="47"/>
+      <c r="O21" s="47"/>
+      <c r="P21" s="47"/>
+    </row>
+    <row r="22" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I22" s="47"/>
+      <c r="J22" s="47"/>
+      <c r="K22" s="47"/>
+      <c r="L22" s="47"/>
+      <c r="M22" s="47"/>
+      <c r="N22" s="47"/>
+      <c r="O22" s="47"/>
+      <c r="P22" s="47"/>
+    </row>
+    <row r="23" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I23" s="47"/>
+      <c r="J23" s="47"/>
+      <c r="K23" s="47"/>
+      <c r="L23" s="47"/>
+      <c r="M23" s="47"/>
+      <c r="N23" s="47"/>
+      <c r="O23" s="47"/>
+      <c r="P23" s="47"/>
+    </row>
+    <row r="24" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I24" s="47"/>
+      <c r="J24" s="47"/>
+      <c r="K24" s="47"/>
+      <c r="L24" s="47"/>
+      <c r="M24" s="47"/>
+      <c r="N24" s="47"/>
+      <c r="O24" s="47"/>
+      <c r="P24" s="47"/>
+    </row>
+    <row r="25" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I25" s="47"/>
+      <c r="J25" s="47"/>
+      <c r="K25" s="47"/>
+      <c r="L25" s="47"/>
+      <c r="M25" s="47"/>
+      <c r="N25" s="47"/>
+      <c r="O25" s="47"/>
+      <c r="P25" s="47"/>
+    </row>
+    <row r="26" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I26" s="47"/>
+      <c r="J26" s="47"/>
+      <c r="K26" s="47"/>
+      <c r="L26" s="47"/>
+      <c r="M26" s="47"/>
+      <c r="N26" s="47"/>
+      <c r="O26" s="47"/>
+      <c r="P26" s="47"/>
+    </row>
+    <row r="27" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I27" s="47"/>
+      <c r="J27" s="47"/>
+      <c r="K27" s="47"/>
+      <c r="L27" s="47"/>
+      <c r="M27" s="47"/>
+      <c r="N27" s="47"/>
+      <c r="O27" s="47"/>
+      <c r="P27" s="47"/>
+    </row>
+    <row r="28" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I28" s="47"/>
+      <c r="J28" s="47"/>
+      <c r="K28" s="47"/>
+      <c r="L28" s="47"/>
+      <c r="M28" s="47"/>
+      <c r="N28" s="47"/>
+      <c r="O28" s="47"/>
+      <c r="P28" s="47"/>
+    </row>
+    <row r="29" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I29" s="47"/>
+      <c r="J29" s="47"/>
+      <c r="K29" s="47"/>
+      <c r="L29" s="47"/>
+      <c r="M29" s="47"/>
+      <c r="N29" s="47"/>
+      <c r="O29" s="47"/>
+      <c r="P29" s="47"/>
+    </row>
+    <row r="30" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
+      <c r="K30" s="47"/>
+      <c r="L30" s="47"/>
+      <c r="M30" s="47"/>
+      <c r="N30" s="47"/>
+      <c r="O30" s="47"/>
+      <c r="P30" s="47"/>
+    </row>
+    <row r="31" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
+      <c r="K31" s="47"/>
+      <c r="L31" s="47"/>
+      <c r="M31" s="47"/>
+      <c r="N31" s="47"/>
+      <c r="O31" s="47"/>
+      <c r="P31" s="47"/>
+    </row>
+    <row r="32" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2109,31 +2174,18 @@
     <row r="992" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="993" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="994" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="995" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="996" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="997" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="998" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="999" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1001" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="O26:O27"/>
-    <mergeCell ref="O28:O29"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
+  <mergeCells count="10">
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -2163,243 +2215,243 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="49"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="47" t="s">
+      <c r="J3" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="48"/>
-      <c r="L3" s="49"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="33"/>
     </row>
     <row r="4" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
     </row>
     <row r="5" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
     </row>
     <row r="6" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
     </row>
     <row r="7" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
     </row>
     <row r="8" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
     </row>
     <row r="9" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
     </row>
     <row r="10" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
     </row>
     <row r="11" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
     </row>
     <row r="12" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
     </row>
     <row r="13" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
     </row>
     <row r="14" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
     </row>
     <row r="15" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="29"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="29"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="25"/>
     </row>
     <row r="16" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Se agrego los Casos de Prueba a la funcionalidad agregar usuario
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M1.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M1.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2b6b49da01230f2/Documentos/proyecto wong/Softgenix-Peru/2-Desarrollo/SCIP/pruebas-calidad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="11_8AF91C39AE0E0FE7D0B96C6DE05857BA94B61638" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8698F2D4-E9EC-441A-9427-513FEC1186EC}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="11_8AF91C39AE0E0FE7D0B96C6DE05857BA94B61638" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD896295-2151-4D88-87AC-558CFD71B197}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="7320" yWindow="3630" windowWidth="17925" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clase equivalencia categoria" sheetId="1" r:id="rId1"/>
-    <sheet name="2.0CP categoria" sheetId="2" r:id="rId2"/>
+    <sheet name="CP Agregar categoria" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -46,12 +46,6 @@
     <t>Código</t>
   </si>
   <si>
-    <t>AGREGAR USUARIO</t>
-  </si>
-  <si>
-    <t>CONDICIONES DE ENTRADA</t>
-  </si>
-  <si>
     <t>Caso prueba</t>
   </si>
   <si>
@@ -61,21 +55,6 @@
     <t>Clases de equivalencia</t>
   </si>
   <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Usuario</t>
-  </si>
-  <si>
-    <t>Contraseña</t>
-  </si>
-  <si>
-    <t>Tipo de Perfil</t>
-  </si>
-  <si>
-    <t>Foto</t>
-  </si>
-  <si>
     <t>Resultado esperado</t>
   </si>
   <si>
@@ -100,24 +79,6 @@
     <t>CP06</t>
   </si>
   <si>
-    <t>CP07</t>
-  </si>
-  <si>
-    <t>CP08</t>
-  </si>
-  <si>
-    <t>CP09</t>
-  </si>
-  <si>
-    <t>CP10</t>
-  </si>
-  <si>
-    <t>CP11</t>
-  </si>
-  <si>
-    <t>CP12</t>
-  </si>
-  <si>
     <t>Identificador</t>
   </si>
   <si>
@@ -194,30 +155,72 @@
   </si>
   <si>
     <t>CEV&lt;05&gt;</t>
+  </si>
+  <si>
+    <t>AGREGAR CATEGORIA</t>
+  </si>
+  <si>
+    <t>CONDICIONES DE  ENTRADA</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>agregado exitoso</t>
+  </si>
+  <si>
+    <t>CEV&lt;03&gt;,CEV&lt;04&gt;CEV&lt;05&gt;</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>casacas</t>
+  </si>
+  <si>
+    <t>Agregado correctamente</t>
+  </si>
+  <si>
+    <t>Agregado Correctamente</t>
+  </si>
+  <si>
+    <t>CASACAS</t>
+  </si>
+  <si>
+    <t>Agregar con descripcion incorrecta</t>
+  </si>
+  <si>
+    <t>CEV&lt;03&gt;,CEV&lt;05&gt;CENV&lt;05&gt;</t>
+  </si>
+  <si>
+    <t>registro fallido</t>
+  </si>
+  <si>
+    <t>CEV&lt;03&gt;,CEV&lt;05&gt;CENV&lt;04&gt;</t>
+  </si>
+  <si>
+    <t>c@saca</t>
+  </si>
+  <si>
+    <t>CEV&lt;03&gt;,CEV&lt;05&gt;CENV&lt;06&gt;</t>
+  </si>
+  <si>
+    <t>ASDFFDSDSFDFDGDSDFSDSDFSDFSDFDSFFFSDDFFFDSSDFDSGSDESDFSDFFSDFSDFSD</t>
+  </si>
+  <si>
+    <t>ERROR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -229,31 +232,6 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -281,8 +259,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -321,81 +320,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE6B8AF"/>
-        <bgColor rgb="FFE6B8AF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF9CB9C"/>
-        <bgColor rgb="FFF9CB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9FC5E8"/>
-        <bgColor rgb="FF9FC5E8"/>
+        <fgColor rgb="FFB1A0C7"/>
+        <bgColor rgb="FFB4A7D6"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="7">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -450,146 +385,136 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{4FE11987-A7A7-4235-AF2D-82033F1DCB3F}"/>
   </cellStyles>
@@ -650,6 +575,61 @@
         <a:xfrm>
           <a:off x="1762125" y="2857500"/>
           <a:ext cx="7772400" cy="4278745"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>590934</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>28647</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88FB49BF-92DF-3FCD-6BDA-B20ABD3C2646}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3876675" y="5057775"/>
+          <a:ext cx="2753109" cy="514422"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -865,7 +845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:P994"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
@@ -887,329 +867,329 @@
     <row r="3" spans="2:16" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="2:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="35" t="s">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="36"/>
-      <c r="G5" s="35" t="s">
+      <c r="F5" s="9"/>
+      <c r="G5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="36"/>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="F6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="G6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="14"/>
+      <c r="D8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="1"/>
+      <c r="C11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C12" s="9"/>
+      <c r="D12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="F12" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="40" t="s">
+      <c r="H12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="G7" s="40" t="s">
+    </row>
+    <row r="13" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="40" t="s">
+      <c r="H13" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="41"/>
-      <c r="D8" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="H8" s="40" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="40" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="44" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="44" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-    </row>
-    <row r="11" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="28"/>
-      <c r="C11" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="H11" s="40" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C12" s="36"/>
-      <c r="D12" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="46" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="H12" s="40" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="H13" s="40" t="s">
-        <v>47</v>
-      </c>
-    </row>
     <row r="14" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I14" s="47"/>
-      <c r="J14" s="47"/>
-      <c r="K14" s="47"/>
-      <c r="L14" s="47"/>
-      <c r="M14" s="47"/>
-      <c r="N14" s="47"/>
-      <c r="O14" s="47"/>
-      <c r="P14" s="47"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
     </row>
     <row r="15" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I15" s="47"/>
-      <c r="J15" s="47"/>
-      <c r="K15" s="47"/>
-      <c r="L15" s="47"/>
-      <c r="M15" s="47"/>
-      <c r="N15" s="47"/>
-      <c r="O15" s="47"/>
-      <c r="P15" s="47"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
     </row>
     <row r="16" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
-      <c r="K16" s="47"/>
-      <c r="L16" s="47"/>
-      <c r="M16" s="47"/>
-      <c r="N16" s="47"/>
-      <c r="O16" s="47"/>
-      <c r="P16" s="47"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
     </row>
     <row r="17" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
-      <c r="K17" s="47"/>
-      <c r="L17" s="47"/>
-      <c r="M17" s="47"/>
-      <c r="N17" s="47"/>
-      <c r="O17" s="47"/>
-      <c r="P17" s="47"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
     </row>
     <row r="18" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
-      <c r="K18" s="47"/>
-      <c r="L18" s="47"/>
-      <c r="M18" s="47"/>
-      <c r="N18" s="47"/>
-      <c r="O18" s="47"/>
-      <c r="P18" s="47"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
     </row>
     <row r="19" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
-      <c r="K19" s="47"/>
-      <c r="L19" s="47"/>
-      <c r="M19" s="47"/>
-      <c r="N19" s="47"/>
-      <c r="O19" s="47"/>
-      <c r="P19" s="47"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
     </row>
     <row r="20" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I20" s="47"/>
-      <c r="J20" s="47"/>
-      <c r="K20" s="47"/>
-      <c r="L20" s="47"/>
-      <c r="M20" s="47"/>
-      <c r="N20" s="47"/>
-      <c r="O20" s="47"/>
-      <c r="P20" s="47"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
     </row>
     <row r="21" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="47"/>
-      <c r="M21" s="47"/>
-      <c r="N21" s="47"/>
-      <c r="O21" s="47"/>
-      <c r="P21" s="47"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
     </row>
     <row r="22" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I22" s="47"/>
-      <c r="J22" s="47"/>
-      <c r="K22" s="47"/>
-      <c r="L22" s="47"/>
-      <c r="M22" s="47"/>
-      <c r="N22" s="47"/>
-      <c r="O22" s="47"/>
-      <c r="P22" s="47"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
     </row>
     <row r="23" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I23" s="47"/>
-      <c r="J23" s="47"/>
-      <c r="K23" s="47"/>
-      <c r="L23" s="47"/>
-      <c r="M23" s="47"/>
-      <c r="N23" s="47"/>
-      <c r="O23" s="47"/>
-      <c r="P23" s="47"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
     </row>
     <row r="24" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I24" s="47"/>
-      <c r="J24" s="47"/>
-      <c r="K24" s="47"/>
-      <c r="L24" s="47"/>
-      <c r="M24" s="47"/>
-      <c r="N24" s="47"/>
-      <c r="O24" s="47"/>
-      <c r="P24" s="47"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
     </row>
     <row r="25" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I25" s="47"/>
-      <c r="J25" s="47"/>
-      <c r="K25" s="47"/>
-      <c r="L25" s="47"/>
-      <c r="M25" s="47"/>
-      <c r="N25" s="47"/>
-      <c r="O25" s="47"/>
-      <c r="P25" s="47"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
     </row>
     <row r="26" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I26" s="47"/>
-      <c r="J26" s="47"/>
-      <c r="K26" s="47"/>
-      <c r="L26" s="47"/>
-      <c r="M26" s="47"/>
-      <c r="N26" s="47"/>
-      <c r="O26" s="47"/>
-      <c r="P26" s="47"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
     </row>
     <row r="27" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I27" s="47"/>
-      <c r="J27" s="47"/>
-      <c r="K27" s="47"/>
-      <c r="L27" s="47"/>
-      <c r="M27" s="47"/>
-      <c r="N27" s="47"/>
-      <c r="O27" s="47"/>
-      <c r="P27" s="47"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
     </row>
     <row r="28" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I28" s="47"/>
-      <c r="J28" s="47"/>
-      <c r="K28" s="47"/>
-      <c r="L28" s="47"/>
-      <c r="M28" s="47"/>
-      <c r="N28" s="47"/>
-      <c r="O28" s="47"/>
-      <c r="P28" s="47"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
     </row>
     <row r="29" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
-      <c r="K29" s="47"/>
-      <c r="L29" s="47"/>
-      <c r="M29" s="47"/>
-      <c r="N29" s="47"/>
-      <c r="O29" s="47"/>
-      <c r="P29" s="47"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
     </row>
     <row r="30" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
-      <c r="K30" s="47"/>
-      <c r="L30" s="47"/>
-      <c r="M30" s="47"/>
-      <c r="N30" s="47"/>
-      <c r="O30" s="47"/>
-      <c r="P30" s="47"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
     </row>
     <row r="31" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I31" s="47"/>
-      <c r="J31" s="47"/>
-      <c r="K31" s="47"/>
-      <c r="L31" s="47"/>
-      <c r="M31" s="47"/>
-      <c r="N31" s="47"/>
-      <c r="O31" s="47"/>
-      <c r="P31" s="47"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
     </row>
     <row r="32" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2176,16 +2156,16 @@
     <row r="994" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -2195,265 +2175,227 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L991"/>
+  <dimension ref="A1:J977"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="35.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="25.42578125" customWidth="1"/>
-    <col min="10" max="28" width="10" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="39" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10" hidden="1" customWidth="1"/>
+    <col min="11" max="28" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+    </row>
+    <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="19"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+    </row>
+    <row r="5" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-    </row>
-    <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="31" t="s">
+      <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="33"/>
-    </row>
-    <row r="3" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="E5" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="H5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+    </row>
+    <row r="6" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="C6" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+    </row>
+    <row r="7" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="C7" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+    </row>
+    <row r="8" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="C8" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="26"/>
+      <c r="G8" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+    </row>
+    <row r="9" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="C9" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="31">
+        <v>14552</v>
+      </c>
+      <c r="G9" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+    </row>
+    <row r="10" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="C10" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+    </row>
+    <row r="11" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="32"/>
-      <c r="L3" s="33"/>
-    </row>
-    <row r="4" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-    </row>
-    <row r="5" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-    </row>
-    <row r="6" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-    </row>
-    <row r="7" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-    </row>
-    <row r="8" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-    </row>
-    <row r="9" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-    </row>
-    <row r="10" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-    </row>
-    <row r="11" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-    </row>
-    <row r="12" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-    </row>
-    <row r="13" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-    </row>
-    <row r="14" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-    </row>
-    <row r="15" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="25"/>
-    </row>
-    <row r="16" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="C11" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+    </row>
+    <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3415,27 +3357,23 @@
     <row r="975" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="976" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="977" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="978" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="979" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="980" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="981" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="982" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="983" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="984" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="985" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="986" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="987" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="988" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="989" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="9">
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H10:J10"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H5:J5"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F10" r:id="rId1" xr:uid="{656304BE-4E34-444D-BBDD-7D1F982BB354}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrego la Clase Equivalencia Modificar Categoria al documento de prueba
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M1.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M1.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2b6b49da01230f2/Documentos/proyecto wong/Softgenix-Peru/2-Desarrollo/SCIP/pruebas-calidad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="106" documentId="11_8AF91C39AE0E0FE7D0B96C6DE05857BA94B61638" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD896295-2151-4D88-87AC-558CFD71B197}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="11_8AF91C39AE0E0FE7D0B96C6DE05857BA94B61638" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BC49721-90C9-467C-9EF3-7BC4168F7804}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clase equivalencia categoria" sheetId="1" r:id="rId1"/>
     <sheet name="CP Agregar categoria" sheetId="2" r:id="rId2"/>
+    <sheet name="CE Modificar Categoria" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="61">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -415,7 +416,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
@@ -436,45 +437,13 @@
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -486,9 +455,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -511,7 +477,48 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -630,6 +637,61 @@
         <a:xfrm>
           <a:off x="3876675" y="5057775"/>
           <a:ext cx="2753109" cy="514422"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>55976</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50EFA591-08EE-1B3D-5C94-C24D98714827}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2019300" y="3695700"/>
+          <a:ext cx="7772400" cy="3780251"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -869,14 +931,14 @@
     <row r="5" spans="2:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="12" t="s">
+      <c r="F5" s="23"/>
+      <c r="G5" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="9"/>
+      <c r="H5" s="23"/>
     </row>
     <row r="6" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="3" t="s">
@@ -899,7 +961,7 @@
       </c>
     </row>
     <row r="7" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="24" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -919,14 +981,14 @@
       </c>
     </row>
     <row r="8" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="14"/>
-      <c r="D8" s="13" t="s">
+      <c r="C8" s="25"/>
+      <c r="D8" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="27" t="s">
         <v>36</v>
       </c>
       <c r="G8" s="6" t="s">
@@ -937,10 +999,10 @@
       </c>
     </row>
     <row r="9" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="6" t="s">
         <v>26</v>
       </c>
@@ -949,8 +1011,8 @@
       </c>
     </row>
     <row r="10" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
       <c r="E10" s="4" t="s">
         <v>37</v>
       </c>
@@ -962,7 +1024,7 @@
     </row>
     <row r="11" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="28" t="s">
         <v>28</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -982,14 +1044,14 @@
       </c>
     </row>
     <row r="12" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C12" s="9"/>
-      <c r="D12" s="8" t="s">
+      <c r="C12" s="23"/>
+      <c r="D12" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="29" t="s">
         <v>42</v>
       </c>
       <c r="G12" s="6" t="s">
@@ -1000,10 +1062,10 @@
       </c>
     </row>
     <row r="13" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
       <c r="G13" s="6" t="s">
         <v>33</v>
       </c>
@@ -2156,16 +2218,16 @@
     <row r="994" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="C7:C10"/>
     <mergeCell ref="D8:D10"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="E5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -2177,7 +2239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J977"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -2197,26 +2259,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="18" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -2228,168 +2290,168 @@
       <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="10" t="s">
         <v>28</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
     </row>
     <row r="6" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="27" t="s">
+      <c r="H6" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
     </row>
     <row r="7" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="24" t="s">
+      <c r="G7" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="27" t="s">
+      <c r="H7" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
     </row>
     <row r="8" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="30" t="s">
+      <c r="F8" s="14"/>
+      <c r="G8" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="H8" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
     </row>
     <row r="9" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="31">
+      <c r="F9" s="18">
         <v>14552</v>
       </c>
-      <c r="G9" s="30" t="s">
+      <c r="G9" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H9" s="27" t="s">
+      <c r="H9" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
     </row>
     <row r="10" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="32" t="s">
+      <c r="F10" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="G10" s="30" t="s">
+      <c r="G10" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H10" s="27" t="s">
+      <c r="H10" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
     </row>
     <row r="11" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="F11" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="G11" s="34" t="s">
+      <c r="G11" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="H11" s="27" t="s">
+      <c r="H11" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
     </row>
     <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3359,15 +3421,15 @@
     <row r="977" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H5:J5"/>
     <mergeCell ref="H11:J11"/>
     <mergeCell ref="H6:J6"/>
     <mergeCell ref="H7:J7"/>
     <mergeCell ref="H8:J8"/>
     <mergeCell ref="H9:J9"/>
     <mergeCell ref="H10:J10"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H5:J5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F10" r:id="rId1" xr:uid="{656304BE-4E34-444D-BBDD-7D1F982BB354}"/>
@@ -3376,4 +3438,118 @@
   <pageSetup orientation="landscape"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98AB587F-8DFE-4C08-940C-DE9938F42560}">
+  <dimension ref="B4:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="23"/>
+      <c r="F4" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="23"/>
+    </row>
+    <row r="5" spans="2:7" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="63" x14ac:dyDescent="0.2">
+      <c r="B6" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="B7" s="23"/>
+      <c r="C7" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C7:C8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrego Casos de Prueba a Modificar categoria
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M1.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M1.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2b6b49da01230f2/Documentos/proyecto wong/Softgenix-Peru/2-Desarrollo/SCIP/pruebas-calidad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="119" documentId="11_8AF91C39AE0E0FE7D0B96C6DE05857BA94B61638" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BC49721-90C9-467C-9EF3-7BC4168F7804}"/>
+  <xr:revisionPtr revIDLastSave="156" documentId="11_8AF91C39AE0E0FE7D0B96C6DE05857BA94B61638" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13757786-FD31-4950-A8A1-A3ABFDE10473}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clase equivalencia categoria" sheetId="1" r:id="rId1"/>
     <sheet name="CP Agregar categoria" sheetId="2" r:id="rId2"/>
     <sheet name="CE Modificar Categoria" sheetId="3" r:id="rId3"/>
+    <sheet name="CP Modificar Categoria" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="66">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -210,13 +211,28 @@
   </si>
   <si>
     <t>ERROR</t>
+  </si>
+  <si>
+    <t>MODIFICAR CATEGORIA</t>
+  </si>
+  <si>
+    <t>modificacion exitoso</t>
+  </si>
+  <si>
+    <t>CEV&lt;01&gt;,CEV&lt;02&gt;</t>
+  </si>
+  <si>
+    <t>Modificado correctamente</t>
+  </si>
+  <si>
+    <t>Modificado Correctamente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -281,8 +297,15 @@
       <name val="Garamond"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,6 +346,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB1A0C7"/>
         <bgColor rgb="FFB4A7D6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor rgb="FFB4A7D6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor rgb="FFB6D7A8"/>
       </patternFill>
     </fill>
   </fills>
@@ -416,7 +451,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
@@ -477,12 +512,24 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -491,18 +538,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -513,11 +548,38 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -931,14 +993,14 @@
     <row r="5" spans="2:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="22" t="s">
+      <c r="F5" s="24"/>
+      <c r="G5" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="23"/>
+      <c r="H5" s="24"/>
     </row>
     <row r="6" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="3" t="s">
@@ -961,7 +1023,7 @@
       </c>
     </row>
     <row r="7" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="28" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -981,14 +1043,14 @@
       </c>
     </row>
     <row r="8" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="25"/>
-      <c r="D8" s="24" t="s">
+      <c r="C8" s="29"/>
+      <c r="D8" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="25" t="s">
         <v>36</v>
       </c>
       <c r="G8" s="6" t="s">
@@ -999,10 +1061,10 @@
       </c>
     </row>
     <row r="9" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
       <c r="G9" s="6" t="s">
         <v>26</v>
       </c>
@@ -1011,8 +1073,8 @@
       </c>
     </row>
     <row r="10" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
       <c r="E10" s="4" t="s">
         <v>37</v>
       </c>
@@ -1024,7 +1086,7 @@
     </row>
     <row r="11" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="23" t="s">
         <v>28</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -1044,14 +1106,14 @@
       </c>
     </row>
     <row r="12" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C12" s="23"/>
-      <c r="D12" s="28" t="s">
+      <c r="C12" s="24"/>
+      <c r="D12" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="29" t="s">
+      <c r="F12" s="26" t="s">
         <v>42</v>
       </c>
       <c r="G12" s="6" t="s">
@@ -1062,10 +1124,10 @@
       </c>
     </row>
     <row r="13" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
       <c r="G13" s="6" t="s">
         <v>33</v>
       </c>
@@ -2218,16 +2280,16 @@
     <row r="994" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -2299,7 +2361,7 @@
       <c r="G5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="27" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="35"/>
@@ -2324,11 +2386,11 @@
       <c r="G6" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
     </row>
     <row r="7" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="11" t="s">
@@ -2349,11 +2411,11 @@
       <c r="G7" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="H7" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
     </row>
     <row r="8" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="15" t="s">
@@ -2372,11 +2434,11 @@
       <c r="G8" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
     </row>
     <row r="9" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="15" t="s">
@@ -2397,11 +2459,11 @@
       <c r="G9" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H9" s="30" t="s">
+      <c r="H9" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
     </row>
     <row r="10" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="15" t="s">
@@ -2422,11 +2484,11 @@
       <c r="G10" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H10" s="30" t="s">
+      <c r="H10" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
     </row>
     <row r="11" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="20" t="s">
@@ -2447,11 +2509,11 @@
       <c r="G11" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="H11" s="30" t="s">
+      <c r="H11" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
     </row>
     <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3444,7 +3506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98AB587F-8DFE-4C08-940C-DE9938F42560}">
   <dimension ref="B4:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
@@ -3459,18 +3521,18 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="22" t="s">
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="22" t="s">
+      <c r="E4" s="24"/>
+      <c r="F4" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="23"/>
-    </row>
-    <row r="5" spans="2:7" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="G4" s="24"/>
+    </row>
+    <row r="5" spans="2:7" ht="31.5" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -3490,8 +3552,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="63" x14ac:dyDescent="0.2">
-      <c r="B6" s="28" t="s">
+    <row r="6" spans="2:7" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="B6" s="23" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -3510,12 +3572,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="B7" s="23"/>
-      <c r="C7" s="28" t="s">
+    <row r="7" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B7" s="24"/>
+      <c r="C7" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="25" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="37" t="s">
@@ -3528,11 +3590,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
+    <row r="8" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
       <c r="F8" s="6" t="s">
         <v>33</v>
       </c>
@@ -3552,4 +3614,238 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03A99724-3612-4138-A39F-D3221CA81224}">
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+    </row>
+    <row r="7" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
+    </row>
+    <row r="8" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="I8" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="I8:K8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrego  los casos de prueba incorrectos a Modificar Categoria
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M1.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2b6b49da01230f2/Documentos/proyecto wong/Softgenix-Peru/2-Desarrollo/SCIP/pruebas-calidad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="156" documentId="11_8AF91C39AE0E0FE7D0B96C6DE05857BA94B61638" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13757786-FD31-4950-A8A1-A3ABFDE10473}"/>
+  <xr:revisionPtr revIDLastSave="163" documentId="11_8AF91C39AE0E0FE7D0B96C6DE05857BA94B61638" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81BFAEE3-EA94-47E4-882D-404EED497A5A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="69">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -226,6 +226,15 @@
   </si>
   <si>
     <t>Modificado Correctamente</t>
+  </si>
+  <si>
+    <t>Modificacion con descripcion incorrecta</t>
+  </si>
+  <si>
+    <t>CEV&lt;02&gt;,CENV&lt;01&gt;</t>
+  </si>
+  <si>
+    <t>CEV&lt;02&gt;,CENV&lt;02&gt;</t>
   </si>
 </sst>
 </file>
@@ -361,7 +370,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -445,13 +454,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
@@ -515,29 +537,50 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -557,29 +600,26 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -993,14 +1033,14 @@
     <row r="5" spans="2:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="24"/>
-      <c r="G5" s="27" t="s">
+      <c r="F5" s="31"/>
+      <c r="G5" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="24"/>
+      <c r="H5" s="31"/>
     </row>
     <row r="6" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="3" t="s">
@@ -1023,7 +1063,7 @@
       </c>
     </row>
     <row r="7" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="32" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1043,14 +1083,14 @@
       </c>
     </row>
     <row r="8" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="29"/>
-      <c r="D8" s="28" t="s">
+      <c r="C8" s="33"/>
+      <c r="D8" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="35" t="s">
         <v>36</v>
       </c>
       <c r="G8" s="6" t="s">
@@ -1061,10 +1101,10 @@
       </c>
     </row>
     <row r="9" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
       <c r="G9" s="6" t="s">
         <v>26</v>
       </c>
@@ -1073,8 +1113,8 @@
       </c>
     </row>
     <row r="10" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
       <c r="E10" s="4" t="s">
         <v>37</v>
       </c>
@@ -1086,7 +1126,7 @@
     </row>
     <row r="11" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="36" t="s">
         <v>28</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -1106,14 +1146,14 @@
       </c>
     </row>
     <row r="12" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C12" s="24"/>
-      <c r="D12" s="23" t="s">
+      <c r="C12" s="31"/>
+      <c r="D12" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="26" t="s">
+      <c r="F12" s="37" t="s">
         <v>42</v>
       </c>
       <c r="G12" s="6" t="s">
@@ -1124,10 +1164,10 @@
       </c>
     </row>
     <row r="13" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
       <c r="G13" s="6" t="s">
         <v>33</v>
       </c>
@@ -2280,16 +2320,16 @@
     <row r="994" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="C7:C10"/>
     <mergeCell ref="D8:D10"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="E5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -2321,11 +2361,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
     </row>
     <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2333,10 +2373,10 @@
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="34"/>
+      <c r="F4" s="41"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -2361,11 +2401,11 @@
       <c r="G5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="27" t="s">
+      <c r="H5" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
     </row>
     <row r="6" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="11" t="s">
@@ -2386,11 +2426,11 @@
       <c r="G6" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="36" t="s">
+      <c r="H6" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
     </row>
     <row r="7" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="11" t="s">
@@ -2411,11 +2451,11 @@
       <c r="G7" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="36" t="s">
+      <c r="H7" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
     </row>
     <row r="8" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="15" t="s">
@@ -2434,11 +2474,11 @@
       <c r="G8" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="36" t="s">
+      <c r="H8" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
     </row>
     <row r="9" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="15" t="s">
@@ -2459,11 +2499,11 @@
       <c r="G9" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H9" s="36" t="s">
+      <c r="H9" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
     </row>
     <row r="10" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="15" t="s">
@@ -2484,11 +2524,11 @@
       <c r="G10" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H10" s="36" t="s">
+      <c r="H10" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
     </row>
     <row r="11" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="20" t="s">
@@ -2509,11 +2549,11 @@
       <c r="G11" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="H11" s="36" t="s">
+      <c r="H11" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="I11" s="36"/>
-      <c r="J11" s="36"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
     </row>
     <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3523,14 +3563,14 @@
     <row r="4" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="24"/>
-      <c r="F4" s="27" t="s">
+      <c r="E4" s="31"/>
+      <c r="F4" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="24"/>
+      <c r="G4" s="31"/>
     </row>
     <row r="5" spans="2:7" ht="31.5" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
@@ -3553,7 +3593,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="36" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -3573,14 +3613,14 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="24"/>
-      <c r="C7" s="23" t="s">
+      <c r="B7" s="31"/>
+      <c r="C7" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="37" t="s">
+      <c r="E7" s="44" t="s">
         <v>36</v>
       </c>
       <c r="F7" s="6" t="s">
@@ -3591,10 +3631,10 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
       <c r="F8" s="6" t="s">
         <v>33</v>
       </c>
@@ -3621,7 +3661,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3691,17 +3731,17 @@
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="3" t="s">
         <v>6</v>
@@ -3712,124 +3752,165 @@
       <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="38" t="s">
+      <c r="E6" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
       <c r="H6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="27" t="s">
+      <c r="I6" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-    </row>
-    <row r="7" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="J6" s="42"/>
+      <c r="K6" s="42"/>
+    </row>
+    <row r="7" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E7" s="38" t="s">
+      <c r="E7" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="40" t="s">
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="I7" s="42" t="s">
+      <c r="I7" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
-    </row>
-    <row r="8" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+    </row>
+    <row r="8" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="D8" s="41" t="s">
+      <c r="D8" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="40" t="s">
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="I8" s="42" t="s">
+      <c r="I8" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+    </row>
+    <row r="9" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="42"/>
-      <c r="K9" s="42"/>
-    </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="50"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="J9" s="48"/>
+      <c r="K9" s="49"/>
+    </row>
+    <row r="10" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
-      <c r="B10" s="43"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="50">
+        <v>14552</v>
+      </c>
+      <c r="F10" s="51"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="J10" s="48"/>
+      <c r="K10" s="49"/>
+    </row>
+    <row r="11" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
-      <c r="B11" s="43"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="42"/>
+      <c r="B11" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="50" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="51"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="J11" s="48"/>
+      <c r="K11" s="49"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
       <c r="H12" s="21"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="42"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="I7:K7"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="I12:K12"/>
     <mergeCell ref="E9:G9"/>
@@ -3838,13 +3919,6 @@
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="I11:K11"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="I8:K8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
se agrego los dasos de prueba erroneos a Modificar Usuario
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M1.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2b6b49da01230f2/Documentos/proyecto wong/Softgenix-Peru/2-Desarrollo/SCIP/pruebas-calidad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="163" documentId="11_8AF91C39AE0E0FE7D0B96C6DE05857BA94B61638" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81BFAEE3-EA94-47E4-882D-404EED497A5A}"/>
+  <xr:revisionPtr revIDLastSave="165" documentId="11_8AF91C39AE0E0FE7D0B96C6DE05857BA94B61638" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46DAF664-50F9-41DB-AD1A-BBECFF3C7F62}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="70">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>CEV&lt;02&gt;,CENV&lt;02&gt;</t>
+  </si>
+  <si>
+    <t>CEV&lt;01&gt;,CENV&lt;03&gt;</t>
   </si>
 </sst>
 </file>
@@ -603,6 +606,15 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -611,15 +623,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -805,8 +808,59 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>648111</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>114361</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39831AE5-EE97-0937-CEFD-A2109D3FA71B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2762250" y="5562600"/>
+          <a:ext cx="2943636" cy="438211"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3661,7 +3715,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3827,17 +3881,17 @@
       <c r="D9" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="50"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="52"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="49"/>
       <c r="H9" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="47" t="s">
+      <c r="I9" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="J9" s="48"/>
-      <c r="K9" s="49"/>
+      <c r="J9" s="51"/>
+      <c r="K9" s="52"/>
     </row>
     <row r="10" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
@@ -3850,19 +3904,19 @@
       <c r="D10" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="50">
+      <c r="E10" s="47">
         <v>14552</v>
       </c>
-      <c r="F10" s="51"/>
-      <c r="G10" s="52"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="49"/>
       <c r="H10" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="I10" s="47" t="s">
+      <c r="I10" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="J10" s="48"/>
-      <c r="K10" s="49"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="52"/>
     </row>
     <row r="11" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
@@ -3875,30 +3929,42 @@
       <c r="D11" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="50" t="s">
+      <c r="E11" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="F11" s="51"/>
-      <c r="G11" s="52"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="49"/>
       <c r="H11" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="I11" s="47" t="s">
+      <c r="I11" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="J11" s="48"/>
-      <c r="K11" s="49"/>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J11" s="51"/>
+      <c r="K11" s="52"/>
+    </row>
+    <row r="12" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="45"/>
+      <c r="B12" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="45" t="s">
+        <v>59</v>
+      </c>
       <c r="F12" s="45"/>
       <c r="G12" s="45"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="46"/>
+      <c r="H12" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="I12" s="46" t="s">
+        <v>60</v>
+      </c>
       <c r="J12" s="46"/>
       <c r="K12" s="46"/>
     </row>
@@ -3921,5 +3987,6 @@
     <mergeCell ref="I11:K11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se agrego la clase equivalencia de Borrar usuario
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M1.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M1.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2b6b49da01230f2/Documentos/proyecto wong/Softgenix-Peru/2-Desarrollo/SCIP/pruebas-calidad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="165" documentId="11_8AF91C39AE0E0FE7D0B96C6DE05857BA94B61638" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46DAF664-50F9-41DB-AD1A-BBECFF3C7F62}"/>
+  <xr:revisionPtr revIDLastSave="181" documentId="11_8AF91C39AE0E0FE7D0B96C6DE05857BA94B61638" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D00728E-756C-4849-A637-B5487CD57A64}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clase equivalencia categoria" sheetId="1" r:id="rId1"/>
     <sheet name="CP Agregar categoria" sheetId="2" r:id="rId2"/>
     <sheet name="CE Modificar Categoria" sheetId="3" r:id="rId3"/>
     <sheet name="CP Modificar Categoria" sheetId="4" r:id="rId4"/>
+    <sheet name="CE Borrar Categoria" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="77">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -238,6 +239,27 @@
   </si>
   <si>
     <t>CEV&lt;01&gt;,CENV&lt;03&gt;</t>
+  </si>
+  <si>
+    <t>Borrar</t>
+  </si>
+  <si>
+    <t>Hacer clic en el botón de borrar</t>
+  </si>
+  <si>
+    <t>No hacer clic en el botón de borrar</t>
+  </si>
+  <si>
+    <t>logico</t>
+  </si>
+  <si>
+    <t>Confirmar la acción de borrado cuando se solicite</t>
+  </si>
+  <si>
+    <t>Hacer clic en un área no interactiva</t>
+  </si>
+  <si>
+    <t>Cancelar la acción de borrado cuando se solicite</t>
   </si>
 </sst>
 </file>
@@ -561,12 +583,21 @@
     <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -575,15 +606,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1087,11 +1109,11 @@
     <row r="5" spans="2:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="34" t="s">
         <v>0</v>
       </c>
       <c r="F5" s="31"/>
-      <c r="G5" s="30" t="s">
+      <c r="G5" s="34" t="s">
         <v>1</v>
       </c>
       <c r="H5" s="31"/>
@@ -1117,7 +1139,7 @@
       </c>
     </row>
     <row r="7" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="35" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1137,14 +1159,14 @@
       </c>
     </row>
     <row r="8" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="33"/>
-      <c r="D8" s="32" t="s">
+      <c r="C8" s="36"/>
+      <c r="D8" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="32" t="s">
         <v>36</v>
       </c>
       <c r="G8" s="6" t="s">
@@ -1155,8 +1177,8 @@
       </c>
     </row>
     <row r="9" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
       <c r="E9" s="31"/>
       <c r="F9" s="31"/>
       <c r="G9" s="6" t="s">
@@ -1167,8 +1189,8 @@
       </c>
     </row>
     <row r="10" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
       <c r="E10" s="4" t="s">
         <v>37</v>
       </c>
@@ -1180,7 +1202,7 @@
     </row>
     <row r="11" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="30" t="s">
         <v>28</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -1201,13 +1223,13 @@
     </row>
     <row r="12" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="31"/>
-      <c r="D12" s="36" t="s">
+      <c r="D12" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="35" t="s">
+      <c r="E12" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="37" t="s">
+      <c r="F12" s="33" t="s">
         <v>42</v>
       </c>
       <c r="G12" s="6" t="s">
@@ -2374,16 +2396,16 @@
     <row r="994" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -2455,7 +2477,7 @@
       <c r="G5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="30" t="s">
+      <c r="H5" s="34" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="42"/>
@@ -3617,11 +3639,11 @@
     <row r="4" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="31"/>
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="34" t="s">
         <v>1</v>
       </c>
       <c r="G4" s="31"/>
@@ -3647,7 +3669,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="30" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -3668,10 +3690,10 @@
     </row>
     <row r="7" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B7" s="31"/>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="32" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="44" t="s">
@@ -3714,7 +3736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03A99724-3612-4138-A39F-D3221CA81224}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
@@ -3785,11 +3807,11 @@
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -3814,7 +3836,7 @@
       <c r="H6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="30" t="s">
+      <c r="I6" s="34" t="s">
         <v>10</v>
       </c>
       <c r="J6" s="42"/>
@@ -3970,13 +3992,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="I7:K7"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="I12:K12"/>
     <mergeCell ref="E9:G9"/>
@@ -3985,8 +4000,128 @@
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="I11:K11"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="I7:K7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC91C84-8615-445C-BDE0-542314D70F6C}">
+  <dimension ref="C7:H11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="6.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1"/>
+    <col min="5" max="5" width="33.85546875" customWidth="1"/>
+    <col min="7" max="7" width="35" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="3:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="31"/>
+      <c r="G7" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="31"/>
+    </row>
+    <row r="8" spans="3:8" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="C8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="31"/>
+      <c r="D10" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="E7:F7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se actualizo la clase equivalencia de Borrar usuario
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M1.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2b6b49da01230f2/Documentos/proyecto wong/Softgenix-Peru/2-Desarrollo/SCIP/pruebas-calidad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="181" documentId="11_8AF91C39AE0E0FE7D0B96C6DE05857BA94B61638" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D00728E-756C-4849-A637-B5487CD57A64}"/>
+  <xr:revisionPtr revIDLastSave="182" documentId="11_8AF91C39AE0E0FE7D0B96C6DE05857BA94B61638" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{863C541F-91D2-4C1C-8459-9C2B925E7EFD}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -583,29 +583,29 @@
     <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -885,6 +885,65 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>100784</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BAADC8E-EB95-2FD0-E1C7-9C42F44EF0CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2514600" y="4152900"/>
+          <a:ext cx="7772400" cy="4634684"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -1109,11 +1168,11 @@
     <row r="5" spans="2:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="34" t="s">
+      <c r="E5" s="30" t="s">
         <v>0</v>
       </c>
       <c r="F5" s="31"/>
-      <c r="G5" s="34" t="s">
+      <c r="G5" s="30" t="s">
         <v>1</v>
       </c>
       <c r="H5" s="31"/>
@@ -1139,7 +1198,7 @@
       </c>
     </row>
     <row r="7" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="32" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1159,14 +1218,14 @@
       </c>
     </row>
     <row r="8" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="36"/>
-      <c r="D8" s="35" t="s">
+      <c r="C8" s="33"/>
+      <c r="D8" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="35" t="s">
         <v>36</v>
       </c>
       <c r="G8" s="6" t="s">
@@ -1177,8 +1236,8 @@
       </c>
     </row>
     <row r="9" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
       <c r="E9" s="31"/>
       <c r="F9" s="31"/>
       <c r="G9" s="6" t="s">
@@ -1189,8 +1248,8 @@
       </c>
     </row>
     <row r="10" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
       <c r="E10" s="4" t="s">
         <v>37</v>
       </c>
@@ -1202,7 +1261,7 @@
     </row>
     <row r="11" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="36" t="s">
         <v>28</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -1223,13 +1282,13 @@
     </row>
     <row r="12" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="31"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="32" t="s">
+      <c r="E12" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="33" t="s">
+      <c r="F12" s="37" t="s">
         <v>42</v>
       </c>
       <c r="G12" s="6" t="s">
@@ -2396,16 +2455,16 @@
     <row r="994" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="C7:C10"/>
     <mergeCell ref="D8:D10"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="E5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -2477,7 +2536,7 @@
       <c r="G5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="34" t="s">
+      <c r="H5" s="30" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="42"/>
@@ -3639,11 +3698,11 @@
     <row r="4" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="30" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="31"/>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="30" t="s">
         <v>1</v>
       </c>
       <c r="G4" s="31"/>
@@ -3669,7 +3728,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="36" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -3690,10 +3749,10 @@
     </row>
     <row r="7" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B7" s="31"/>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="35" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="44" t="s">
@@ -3807,11 +3866,11 @@
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="34" t="s">
+      <c r="E5" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -3836,7 +3895,7 @@
       <c r="H6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="34" t="s">
+      <c r="I6" s="30" t="s">
         <v>10</v>
       </c>
       <c r="J6" s="42"/>
@@ -3992,6 +4051,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="I7:K7"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="I12:K12"/>
     <mergeCell ref="E9:G9"/>
@@ -4000,13 +4066,6 @@
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="I11:K11"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="I7:K7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4018,7 +4077,7 @@
   <dimension ref="C7:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4034,16 +4093,16 @@
     <row r="7" spans="3:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
-      <c r="E7" s="34" t="s">
+      <c r="E7" s="30" t="s">
         <v>0</v>
       </c>
       <c r="F7" s="31"/>
-      <c r="G7" s="34" t="s">
+      <c r="G7" s="30" t="s">
         <v>1</v>
       </c>
       <c r="H7" s="31"/>
     </row>
-    <row r="8" spans="3:8" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:8" ht="31.5" x14ac:dyDescent="0.2">
       <c r="C8" s="3" t="s">
         <v>2</v>
       </c>
@@ -4064,7 +4123,7 @@
       </c>
     </row>
     <row r="9" spans="3:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="36" t="s">
         <v>70</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -4085,10 +4144,10 @@
     </row>
     <row r="10" spans="3:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="31"/>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="35" t="s">
         <v>74</v>
       </c>
       <c r="F10" s="44" t="s">
@@ -4123,5 +4182,6 @@
     <mergeCell ref="E7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrego los casos de prueba a Borrar Usuario
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M1.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2b6b49da01230f2/Documentos/proyecto wong/Softgenix-Peru/2-Desarrollo/SCIP/pruebas-calidad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="182" documentId="11_8AF91C39AE0E0FE7D0B96C6DE05857BA94B61638" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{863C541F-91D2-4C1C-8459-9C2B925E7EFD}"/>
+  <xr:revisionPtr revIDLastSave="189" documentId="11_8AF91C39AE0E0FE7D0B96C6DE05857BA94B61638" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{935C39F6-A531-48F3-85FC-9A706A830EB1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clase equivalencia categoria" sheetId="1" r:id="rId1"/>
@@ -18,18 +18,19 @@
     <sheet name="CE Modificar Categoria" sheetId="3" r:id="rId3"/>
     <sheet name="CP Modificar Categoria" sheetId="4" r:id="rId4"/>
     <sheet name="CE Borrar Categoria" sheetId="5" r:id="rId5"/>
+    <sheet name="CP Borrar Categoria" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="oCOje7eQ+BNatKuPs7RwyjtQZmaEt8Ox0GG8W65hv9c="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="oCOje7eQ+BNatKuPs7RwyjtQZmaEt8Ox0GG8W65hv9c="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="84">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -260,6 +261,27 @@
   </si>
   <si>
     <t>Cancelar la acción de borrado cuando se solicite</t>
+  </si>
+  <si>
+    <t>BORRAR CATEGORIA</t>
+  </si>
+  <si>
+    <t>borrado exitoso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hacer clic </t>
+  </si>
+  <si>
+    <t>eliminado correctamente</t>
+  </si>
+  <si>
+    <t>borrado fallido</t>
+  </si>
+  <si>
+    <t>no se elimina</t>
+  </si>
+  <si>
+    <t>categoria no se elimina</t>
   </si>
 </sst>
 </file>
@@ -395,7 +417,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -492,13 +514,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
@@ -583,6 +636,15 @@
     <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -644,6 +706,27 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1168,14 +1251,14 @@
     <row r="5" spans="2:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="31"/>
-      <c r="G5" s="30" t="s">
+      <c r="F5" s="34"/>
+      <c r="G5" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="31"/>
+      <c r="H5" s="34"/>
     </row>
     <row r="6" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="3" t="s">
@@ -1198,7 +1281,7 @@
       </c>
     </row>
     <row r="7" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="35" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1218,14 +1301,14 @@
       </c>
     </row>
     <row r="8" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="33"/>
-      <c r="D8" s="32" t="s">
+      <c r="C8" s="36"/>
+      <c r="D8" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="38" t="s">
         <v>36</v>
       </c>
       <c r="G8" s="6" t="s">
@@ -1236,10 +1319,10 @@
       </c>
     </row>
     <row r="9" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="6" t="s">
         <v>26</v>
       </c>
@@ -1248,8 +1331,8 @@
       </c>
     </row>
     <row r="10" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
       <c r="E10" s="4" t="s">
         <v>37</v>
       </c>
@@ -1261,7 +1344,7 @@
     </row>
     <row r="11" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="39" t="s">
         <v>28</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -1281,14 +1364,14 @@
       </c>
     </row>
     <row r="12" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C12" s="31"/>
-      <c r="D12" s="36" t="s">
+      <c r="C12" s="34"/>
+      <c r="D12" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="35" t="s">
+      <c r="E12" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="37" t="s">
+      <c r="F12" s="40" t="s">
         <v>42</v>
       </c>
       <c r="G12" s="6" t="s">
@@ -1299,10 +1382,10 @@
       </c>
     </row>
     <row r="13" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
       <c r="G13" s="6" t="s">
         <v>33</v>
       </c>
@@ -2496,11 +2579,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2508,10 +2591,10 @@
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
-      <c r="E4" s="40" t="s">
+      <c r="E4" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="41"/>
+      <c r="F4" s="44"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -2536,11 +2619,11 @@
       <c r="G5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="30" t="s">
+      <c r="H5" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
     </row>
     <row r="6" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="11" t="s">
@@ -2561,11 +2644,11 @@
       <c r="G6" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="43" t="s">
+      <c r="H6" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
     </row>
     <row r="7" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="11" t="s">
@@ -2586,11 +2669,11 @@
       <c r="G7" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="43" t="s">
+      <c r="H7" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
     </row>
     <row r="8" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="15" t="s">
@@ -2609,11 +2692,11 @@
       <c r="G8" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="43" t="s">
+      <c r="H8" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
     </row>
     <row r="9" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="15" t="s">
@@ -2634,11 +2717,11 @@
       <c r="G9" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H9" s="43" t="s">
+      <c r="H9" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
     </row>
     <row r="10" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="15" t="s">
@@ -2659,11 +2742,11 @@
       <c r="G10" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H10" s="43" t="s">
+      <c r="H10" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
     </row>
     <row r="11" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="20" t="s">
@@ -2684,11 +2767,11 @@
       <c r="G11" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="H11" s="43" t="s">
+      <c r="H11" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
     </row>
     <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3698,14 +3781,14 @@
     <row r="4" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="31"/>
-      <c r="F4" s="30" t="s">
+      <c r="E4" s="34"/>
+      <c r="F4" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="31"/>
+      <c r="G4" s="34"/>
     </row>
     <row r="5" spans="2:7" ht="31.5" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
@@ -3728,7 +3811,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="39" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -3748,14 +3831,14 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="31"/>
-      <c r="C7" s="36" t="s">
+      <c r="B7" s="34"/>
+      <c r="C7" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="44" t="s">
+      <c r="E7" s="47" t="s">
         <v>36</v>
       </c>
       <c r="F7" s="6" t="s">
@@ -3766,10 +3849,10 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
       <c r="F8" s="6" t="s">
         <v>33</v>
       </c>
@@ -3866,11 +3949,11 @@
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -3887,19 +3970,19 @@
       <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="45" t="s">
+      <c r="E6" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
       <c r="H6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="30" t="s">
+      <c r="I6" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="42"/>
-      <c r="K6" s="42"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="45"/>
     </row>
     <row r="7" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
@@ -3912,19 +3995,19 @@
       <c r="D7" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="E7" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
       <c r="H7" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="I7" s="46" t="s">
+      <c r="I7" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
     </row>
     <row r="8" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
@@ -3937,19 +4020,19 @@
       <c r="D8" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E8" s="45" t="s">
+      <c r="E8" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
       <c r="H8" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="I8" s="46" t="s">
+      <c r="I8" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="J8" s="46"/>
-      <c r="K8" s="46"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
     </row>
     <row r="9" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
@@ -3962,17 +4045,17 @@
       <c r="D9" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="47"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="49"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="52"/>
       <c r="H9" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="50" t="s">
+      <c r="I9" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="J9" s="51"/>
-      <c r="K9" s="52"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="55"/>
     </row>
     <row r="10" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
@@ -3985,19 +4068,19 @@
       <c r="D10" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="47">
+      <c r="E10" s="50">
         <v>14552</v>
       </c>
-      <c r="F10" s="48"/>
-      <c r="G10" s="49"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="52"/>
       <c r="H10" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="I10" s="50" t="s">
+      <c r="I10" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="J10" s="51"/>
-      <c r="K10" s="52"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="55"/>
     </row>
     <row r="11" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
@@ -4010,19 +4093,19 @@
       <c r="D11" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="47" t="s">
+      <c r="E11" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="F11" s="48"/>
-      <c r="G11" s="49"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="52"/>
       <c r="H11" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="I11" s="50" t="s">
+      <c r="I11" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="J11" s="51"/>
-      <c r="K11" s="52"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="55"/>
     </row>
     <row r="12" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
@@ -4035,19 +4118,19 @@
       <c r="D12" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E12" s="45" t="s">
+      <c r="E12" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
       <c r="H12" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="I12" s="46" t="s">
+      <c r="I12" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="J12" s="46"/>
-      <c r="K12" s="46"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -4076,7 +4159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC91C84-8615-445C-BDE0-542314D70F6C}">
   <dimension ref="C7:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -4093,14 +4176,14 @@
     <row r="7" spans="3:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="F7" s="31"/>
-      <c r="G7" s="30" t="s">
+      <c r="F7" s="34"/>
+      <c r="G7" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="31"/>
+      <c r="H7" s="34"/>
     </row>
     <row r="8" spans="3:8" ht="31.5" x14ac:dyDescent="0.2">
       <c r="C8" s="3" t="s">
@@ -4123,7 +4206,7 @@
       </c>
     </row>
     <row r="9" spans="3:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="39" t="s">
         <v>70</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -4143,14 +4226,14 @@
       </c>
     </row>
     <row r="10" spans="3:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="31"/>
-      <c r="D10" s="36" t="s">
+      <c r="C10" s="34"/>
+      <c r="D10" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="44" t="s">
+      <c r="F10" s="47" t="s">
         <v>36</v>
       </c>
       <c r="G10" s="6" t="s">
@@ -4161,10 +4244,10 @@
       </c>
     </row>
     <row r="11" spans="3:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="6" t="s">
         <v>76</v>
       </c>
@@ -4184,4 +4267,243 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5245103-A33C-4B19-AC86-B282B10A8938}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="25.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="56"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+    </row>
+    <row r="7" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="45"/>
+      <c r="K7" s="45"/>
+    </row>
+    <row r="8" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="57" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="58"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="I8" s="60" t="s">
+        <v>80</v>
+      </c>
+      <c r="J8" s="61"/>
+      <c r="K8" s="62"/>
+    </row>
+    <row r="9" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="I9" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+    </row>
+    <row r="10" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="I10" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="J10" s="46"/>
+      <c r="K10" s="46"/>
+    </row>
+    <row r="11" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="I11" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="J11" s="46"/>
+      <c r="K11" s="46"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="I11:K11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se actualizo la casos de prueba de Borrar Categoria
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M1.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2b6b49da01230f2/Documentos/proyecto wong/Softgenix-Peru/2-Desarrollo/SCIP/pruebas-calidad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="189" documentId="11_8AF91C39AE0E0FE7D0B96C6DE05857BA94B61638" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{935C39F6-A531-48F3-85FC-9A706A830EB1}"/>
+  <xr:revisionPtr revIDLastSave="190" documentId="11_8AF91C39AE0E0FE7D0B96C6DE05857BA94B61638" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF35BC64-95FD-40A5-872E-81675D0A4ADE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -645,12 +645,21 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -659,15 +668,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1023,6 +1023,61 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1086427</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>123933</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44F4919C-4C01-CA3B-B06D-EF6454A319B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2286000" y="4286250"/>
+          <a:ext cx="4134427" cy="771633"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
@@ -1251,11 +1306,11 @@
     <row r="5" spans="2:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="37" t="s">
         <v>0</v>
       </c>
       <c r="F5" s="34"/>
-      <c r="G5" s="33" t="s">
+      <c r="G5" s="37" t="s">
         <v>1</v>
       </c>
       <c r="H5" s="34"/>
@@ -1281,7 +1336,7 @@
       </c>
     </row>
     <row r="7" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="38" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1301,14 +1356,14 @@
       </c>
     </row>
     <row r="8" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="36"/>
-      <c r="D8" s="35" t="s">
+      <c r="C8" s="39"/>
+      <c r="D8" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="38" t="s">
+      <c r="F8" s="35" t="s">
         <v>36</v>
       </c>
       <c r="G8" s="6" t="s">
@@ -1319,8 +1374,8 @@
       </c>
     </row>
     <row r="9" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
       <c r="E9" s="34"/>
       <c r="F9" s="34"/>
       <c r="G9" s="6" t="s">
@@ -1331,8 +1386,8 @@
       </c>
     </row>
     <row r="10" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
       <c r="E10" s="4" t="s">
         <v>37</v>
       </c>
@@ -1344,7 +1399,7 @@
     </row>
     <row r="11" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="33" t="s">
         <v>28</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -1365,13 +1420,13 @@
     </row>
     <row r="12" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="34"/>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="38" t="s">
+      <c r="E12" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="40" t="s">
+      <c r="F12" s="36" t="s">
         <v>42</v>
       </c>
       <c r="G12" s="6" t="s">
@@ -2538,16 +2593,16 @@
     <row r="994" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -2619,7 +2674,7 @@
       <c r="G5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="33" t="s">
+      <c r="H5" s="37" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="45"/>
@@ -3781,11 +3836,11 @@
     <row r="4" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="37" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="34"/>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="37" t="s">
         <v>1</v>
       </c>
       <c r="G4" s="34"/>
@@ -3811,7 +3866,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="33" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -3832,10 +3887,10 @@
     </row>
     <row r="7" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B7" s="34"/>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="D7" s="35" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="47" t="s">
@@ -3949,11 +4004,11 @@
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -3978,7 +4033,7 @@
       <c r="H6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="33" t="s">
+      <c r="I6" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J6" s="45"/>
@@ -4134,13 +4189,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="I7:K7"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="I12:K12"/>
     <mergeCell ref="E9:G9"/>
@@ -4149,6 +4197,13 @@
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="I11:K11"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="I7:K7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4176,11 +4231,11 @@
     <row r="7" spans="3:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="37" t="s">
         <v>0</v>
       </c>
       <c r="F7" s="34"/>
-      <c r="G7" s="33" t="s">
+      <c r="G7" s="37" t="s">
         <v>1</v>
       </c>
       <c r="H7" s="34"/>
@@ -4206,7 +4261,7 @@
       </c>
     </row>
     <row r="9" spans="3:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="33" t="s">
         <v>70</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -4227,10 +4282,10 @@
     </row>
     <row r="10" spans="3:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="34"/>
-      <c r="D10" s="39" t="s">
+      <c r="D10" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="E10" s="38" t="s">
+      <c r="E10" s="35" t="s">
         <v>74</v>
       </c>
       <c r="F10" s="47" t="s">
@@ -4274,7 +4329,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4354,11 +4409,11 @@
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
@@ -4383,7 +4438,7 @@
       <c r="H7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="33" t="s">
+      <c r="I7" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J7" s="45"/>
@@ -4491,19 +4546,20 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="I11:K11"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="I7:K7"/>
     <mergeCell ref="E8:G8"/>
     <mergeCell ref="I8:K8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="I11:K11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrego una tabla de resultados para la funcionalidad Categoria
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M1.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2b6b49da01230f2/Documentos/proyecto wong/Softgenix-Peru/2-Desarrollo/SCIP/pruebas-calidad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="190" documentId="11_8AF91C39AE0E0FE7D0B96C6DE05857BA94B61638" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF35BC64-95FD-40A5-872E-81675D0A4ADE}"/>
+  <xr:revisionPtr revIDLastSave="202" documentId="11_8AF91C39AE0E0FE7D0B96C6DE05857BA94B61638" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BEEF798-BFED-4256-B76B-2ED640CEE8B4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clase equivalencia categoria" sheetId="1" r:id="rId1"/>
@@ -19,18 +19,30 @@
     <sheet name="CP Modificar Categoria" sheetId="4" r:id="rId4"/>
     <sheet name="CE Borrar Categoria" sheetId="5" r:id="rId5"/>
     <sheet name="CP Borrar Categoria" sheetId="6" r:id="rId6"/>
+    <sheet name="Resultados F. Categoria" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="oCOje7eQ+BNatKuPs7RwyjtQZmaEt8Ox0GG8W65hv9c="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="oCOje7eQ+BNatKuPs7RwyjtQZmaEt8Ox0GG8W65hv9c="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="95">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -282,13 +294,46 @@
   </si>
   <si>
     <t>categoria no se elimina</t>
+  </si>
+  <si>
+    <t>Funcionalidad</t>
+  </si>
+  <si>
+    <t>Casos de pruebas no válidadas</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Porcentaje con defectos</t>
+  </si>
+  <si>
+    <t>Porcentaje sin defectos</t>
+  </si>
+  <si>
+    <t>Con Defectos</t>
+  </si>
+  <si>
+    <t>Sin Defectos</t>
+  </si>
+  <si>
+    <t>Agregar categoria</t>
+  </si>
+  <si>
+    <t>modificar categoria</t>
+  </si>
+  <si>
+    <t>eliminar categoria</t>
+  </si>
+  <si>
+    <t>Caso de pruebas validadas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -360,8 +405,15 @@
       <name val="Garamond"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -414,6 +466,12 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor rgb="FFB6D7A8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -546,12 +604,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
@@ -645,29 +704,29 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -729,11 +788,27 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{4FE11987-A7A7-4235-AF2D-82033F1DCB3F}"/>
+    <cellStyle name="Porcentaje" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1306,11 +1381,11 @@
     <row r="5" spans="2:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="33" t="s">
         <v>0</v>
       </c>
       <c r="F5" s="34"/>
-      <c r="G5" s="37" t="s">
+      <c r="G5" s="33" t="s">
         <v>1</v>
       </c>
       <c r="H5" s="34"/>
@@ -1336,7 +1411,7 @@
       </c>
     </row>
     <row r="7" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="35" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1356,14 +1431,14 @@
       </c>
     </row>
     <row r="8" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="39"/>
-      <c r="D8" s="38" t="s">
+      <c r="C8" s="36"/>
+      <c r="D8" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="38" t="s">
         <v>36</v>
       </c>
       <c r="G8" s="6" t="s">
@@ -1374,8 +1449,8 @@
       </c>
     </row>
     <row r="9" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
       <c r="E9" s="34"/>
       <c r="F9" s="34"/>
       <c r="G9" s="6" t="s">
@@ -1386,8 +1461,8 @@
       </c>
     </row>
     <row r="10" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
       <c r="E10" s="4" t="s">
         <v>37</v>
       </c>
@@ -1399,7 +1474,7 @@
     </row>
     <row r="11" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="39" t="s">
         <v>28</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -1420,13 +1495,13 @@
     </row>
     <row r="12" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="34"/>
-      <c r="D12" s="33" t="s">
+      <c r="D12" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="35" t="s">
+      <c r="E12" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="36" t="s">
+      <c r="F12" s="40" t="s">
         <v>42</v>
       </c>
       <c r="G12" s="6" t="s">
@@ -2593,16 +2668,16 @@
     <row r="994" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="C7:C10"/>
     <mergeCell ref="D8:D10"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="E5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -2674,7 +2749,7 @@
       <c r="G5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="37" t="s">
+      <c r="H5" s="33" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="45"/>
@@ -3836,11 +3911,11 @@
     <row r="4" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="33" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="34"/>
-      <c r="F4" s="37" t="s">
+      <c r="F4" s="33" t="s">
         <v>1</v>
       </c>
       <c r="G4" s="34"/>
@@ -3866,7 +3941,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="39" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -3887,10 +3962,10 @@
     </row>
     <row r="7" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B7" s="34"/>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="38" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="47" t="s">
@@ -4004,11 +4079,11 @@
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -4033,7 +4108,7 @@
       <c r="H6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="37" t="s">
+      <c r="I6" s="33" t="s">
         <v>10</v>
       </c>
       <c r="J6" s="45"/>
@@ -4189,6 +4264,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="I7:K7"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="I12:K12"/>
     <mergeCell ref="E9:G9"/>
@@ -4197,13 +4279,6 @@
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="I11:K11"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="I7:K7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4231,11 +4306,11 @@
     <row r="7" spans="3:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
-      <c r="E7" s="37" t="s">
+      <c r="E7" s="33" t="s">
         <v>0</v>
       </c>
       <c r="F7" s="34"/>
-      <c r="G7" s="37" t="s">
+      <c r="G7" s="33" t="s">
         <v>1</v>
       </c>
       <c r="H7" s="34"/>
@@ -4261,7 +4336,7 @@
       </c>
     </row>
     <row r="9" spans="3:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="39" t="s">
         <v>70</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -4282,10 +4357,10 @@
     </row>
     <row r="10" spans="3:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="34"/>
-      <c r="D10" s="33" t="s">
+      <c r="D10" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="38" t="s">
         <v>74</v>
       </c>
       <c r="F10" s="47" t="s">
@@ -4328,7 +4403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5245103-A33C-4B19-AC86-B282B10A8938}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -4409,11 +4484,11 @@
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
@@ -4438,7 +4513,7 @@
       <c r="H7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="37" t="s">
+      <c r="I7" s="33" t="s">
         <v>10</v>
       </c>
       <c r="J7" s="45"/>
@@ -4546,20 +4621,172 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="I8:K8"/>
     <mergeCell ref="E9:G9"/>
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="E10:G10"/>
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="I11:K11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="I8:K8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9804A779-B889-4EF9-82E6-958056C46898}">
+  <dimension ref="B5:H10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="63" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="63" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" s="63" t="s">
+        <v>86</v>
+      </c>
+      <c r="G5" s="63" t="s">
+        <v>87</v>
+      </c>
+      <c r="H5" s="63" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+    </row>
+    <row r="7" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="63"/>
+      <c r="C7" s="64" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
+    </row>
+    <row r="8" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B8" s="65" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="66">
+        <v>3</v>
+      </c>
+      <c r="D8" s="66">
+        <v>2</v>
+      </c>
+      <c r="E8" s="66">
+        <v>1</v>
+      </c>
+      <c r="F8" s="66">
+        <f>SUM(C8:E8)</f>
+        <v>6</v>
+      </c>
+      <c r="G8" s="67">
+        <f>C8/F8</f>
+        <v>0.5</v>
+      </c>
+      <c r="H8" s="67">
+        <f>D8/F8</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="66">
+        <v>3</v>
+      </c>
+      <c r="D9" s="66">
+        <v>3</v>
+      </c>
+      <c r="E9" s="66">
+        <v>0</v>
+      </c>
+      <c r="F9" s="66">
+        <f>SUM(C9:E9)</f>
+        <v>6</v>
+      </c>
+      <c r="G9" s="67">
+        <f t="shared" ref="G9:G10" si="0">C9/F9</f>
+        <v>0.5</v>
+      </c>
+      <c r="H9" s="67">
+        <f t="shared" ref="H9:H10" si="1">D9/F9</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B10" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="66">
+        <v>0</v>
+      </c>
+      <c r="D10" s="66">
+        <v>4</v>
+      </c>
+      <c r="E10" s="66">
+        <v>0</v>
+      </c>
+      <c r="F10" s="66">
+        <f>SUM(C10:E10)</f>
+        <v>4</v>
+      </c>
+      <c r="G10" s="67">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="67">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:D6"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="H5:H7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se actualizo una tabla de resultados para la funcionalidad Categoria
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M1.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2b6b49da01230f2/Documentos/proyecto wong/Softgenix-Peru/2-Desarrollo/SCIP/pruebas-calidad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="202" documentId="11_8AF91C39AE0E0FE7D0B96C6DE05857BA94B61638" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BEEF798-BFED-4256-B76B-2ED640CEE8B4}"/>
+  <xr:revisionPtr revIDLastSave="206" documentId="11_8AF91C39AE0E0FE7D0B96C6DE05857BA94B61638" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41F47B42-7DBF-447E-87B4-A5E4120325B8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -704,12 +704,33 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -718,15 +739,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -790,18 +802,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -821,6 +821,903 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Resultados F. Categoria'!$G$5:$G$7</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Porcentaje con defectos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Resultados F. Categoria'!$B$8:$B$10</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Agregar categoria</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>modificar categoria</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>eliminar categoria</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Resultados F. Categoria'!$G$8:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0655-4FDB-83E6-9C152C8BB422}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Resultados F. Categoria'!$H$5:$H$7</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Porcentaje sin defectos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Resultados F. Categoria'!$B$8:$B$10</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Agregar categoria</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>modificar categoria</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>eliminar categoria</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Resultados F. Categoria'!$H$8:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0655-4FDB-83E6-9C152C8BB422}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1392944975"/>
+        <c:axId val="1392944015"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1392944975"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1392944015"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1392944015"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1392944975"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-PE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-PE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1153,6 +2050,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3C9A9BB-0D94-2E19-059E-572C56CAEF7E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
@@ -1381,14 +2319,14 @@
     <row r="5" spans="2:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="34"/>
-      <c r="G5" s="33" t="s">
+      <c r="F5" s="38"/>
+      <c r="G5" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="34"/>
+      <c r="H5" s="38"/>
     </row>
     <row r="6" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="3" t="s">
@@ -1411,7 +2349,7 @@
       </c>
     </row>
     <row r="7" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="42" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1431,14 +2369,14 @@
       </c>
     </row>
     <row r="8" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="36"/>
-      <c r="D8" s="35" t="s">
+      <c r="C8" s="43"/>
+      <c r="D8" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="38" t="s">
+      <c r="F8" s="39" t="s">
         <v>36</v>
       </c>
       <c r="G8" s="6" t="s">
@@ -1449,10 +2387,10 @@
       </c>
     </row>
     <row r="9" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
       <c r="G9" s="6" t="s">
         <v>26</v>
       </c>
@@ -1461,8 +2399,8 @@
       </c>
     </row>
     <row r="10" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
       <c r="E10" s="4" t="s">
         <v>37</v>
       </c>
@@ -1474,7 +2412,7 @@
     </row>
     <row r="11" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="37" t="s">
         <v>28</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -1494,11 +2432,11 @@
       </c>
     </row>
     <row r="12" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C12" s="34"/>
-      <c r="D12" s="39" t="s">
+      <c r="C12" s="38"/>
+      <c r="D12" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="38" t="s">
+      <c r="E12" s="39" t="s">
         <v>30</v>
       </c>
       <c r="F12" s="40" t="s">
@@ -1512,10 +2450,10 @@
       </c>
     </row>
     <row r="13" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
       <c r="G13" s="6" t="s">
         <v>33</v>
       </c>
@@ -2668,16 +3606,16 @@
     <row r="994" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -2709,11 +3647,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
     </row>
     <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2721,10 +3659,10 @@
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
-      <c r="E4" s="43" t="s">
+      <c r="E4" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="44"/>
+      <c r="F4" s="48"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -2749,11 +3687,11 @@
       <c r="G5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="33" t="s">
+      <c r="H5" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
     </row>
     <row r="6" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="11" t="s">
@@ -2774,11 +3712,11 @@
       <c r="G6" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="46" t="s">
+      <c r="H6" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
     </row>
     <row r="7" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="11" t="s">
@@ -2799,11 +3737,11 @@
       <c r="G7" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="46" t="s">
+      <c r="H7" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
     </row>
     <row r="8" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="15" t="s">
@@ -2822,11 +3760,11 @@
       <c r="G8" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="46" t="s">
+      <c r="H8" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="I8" s="46"/>
-      <c r="J8" s="46"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
     </row>
     <row r="9" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="15" t="s">
@@ -2847,11 +3785,11 @@
       <c r="G9" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H9" s="46" t="s">
+      <c r="H9" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="I9" s="46"/>
-      <c r="J9" s="46"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
     </row>
     <row r="10" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="15" t="s">
@@ -2872,11 +3810,11 @@
       <c r="G10" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H10" s="46" t="s">
+      <c r="H10" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="I10" s="46"/>
-      <c r="J10" s="46"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="50"/>
     </row>
     <row r="11" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="20" t="s">
@@ -2897,11 +3835,11 @@
       <c r="G11" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="H11" s="46" t="s">
+      <c r="H11" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
     </row>
     <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3911,14 +4849,14 @@
     <row r="4" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="34"/>
-      <c r="F4" s="33" t="s">
+      <c r="E4" s="38"/>
+      <c r="F4" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="34"/>
+      <c r="G4" s="38"/>
     </row>
     <row r="5" spans="2:7" ht="31.5" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
@@ -3941,7 +4879,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="37" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -3961,14 +4899,14 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="34"/>
-      <c r="C7" s="39" t="s">
+      <c r="B7" s="38"/>
+      <c r="C7" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="D7" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="47" t="s">
+      <c r="E7" s="51" t="s">
         <v>36</v>
       </c>
       <c r="F7" s="6" t="s">
@@ -3979,10 +4917,10 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
       <c r="F8" s="6" t="s">
         <v>33</v>
       </c>
@@ -4079,11 +5017,11 @@
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -4100,19 +5038,19 @@
       <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="48" t="s">
+      <c r="E6" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
       <c r="H6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="33" t="s">
+      <c r="I6" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
     </row>
     <row r="7" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
@@ -4125,19 +5063,19 @@
       <c r="D7" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E7" s="48" t="s">
+      <c r="E7" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
       <c r="H7" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="I7" s="49" t="s">
+      <c r="I7" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
     </row>
     <row r="8" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
@@ -4150,19 +5088,19 @@
       <c r="D8" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E8" s="48" t="s">
+      <c r="E8" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
       <c r="H8" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="I8" s="49" t="s">
+      <c r="I8" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="J8" s="49"/>
-      <c r="K8" s="49"/>
+      <c r="J8" s="53"/>
+      <c r="K8" s="53"/>
     </row>
     <row r="9" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
@@ -4175,17 +5113,17 @@
       <c r="D9" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="50"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="52"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="56"/>
       <c r="H9" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="53" t="s">
+      <c r="I9" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="J9" s="54"/>
-      <c r="K9" s="55"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="59"/>
     </row>
     <row r="10" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
@@ -4198,19 +5136,19 @@
       <c r="D10" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="50">
+      <c r="E10" s="54">
         <v>14552</v>
       </c>
-      <c r="F10" s="51"/>
-      <c r="G10" s="52"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="56"/>
       <c r="H10" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="I10" s="53" t="s">
+      <c r="I10" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="J10" s="54"/>
-      <c r="K10" s="55"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="59"/>
     </row>
     <row r="11" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
@@ -4223,19 +5161,19 @@
       <c r="D11" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="50" t="s">
+      <c r="E11" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="F11" s="51"/>
-      <c r="G11" s="52"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="56"/>
       <c r="H11" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="I11" s="53" t="s">
+      <c r="I11" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="J11" s="54"/>
-      <c r="K11" s="55"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="59"/>
     </row>
     <row r="12" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
@@ -4248,29 +5186,22 @@
       <c r="D12" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E12" s="48" t="s">
+      <c r="E12" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
       <c r="H12" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="I12" s="49" t="s">
+      <c r="I12" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="J12" s="49"/>
-      <c r="K12" s="49"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="I7:K7"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="I12:K12"/>
     <mergeCell ref="E9:G9"/>
@@ -4279,6 +5210,13 @@
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="I11:K11"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="I7:K7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4306,14 +5244,14 @@
     <row r="7" spans="3:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="F7" s="34"/>
-      <c r="G7" s="33" t="s">
+      <c r="F7" s="38"/>
+      <c r="G7" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="34"/>
+      <c r="H7" s="38"/>
     </row>
     <row r="8" spans="3:8" ht="31.5" x14ac:dyDescent="0.2">
       <c r="C8" s="3" t="s">
@@ -4336,7 +5274,7 @@
       </c>
     </row>
     <row r="9" spans="3:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="37" t="s">
         <v>70</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -4356,14 +5294,14 @@
       </c>
     </row>
     <row r="10" spans="3:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="34"/>
-      <c r="D10" s="39" t="s">
+      <c r="C10" s="38"/>
+      <c r="D10" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="E10" s="38" t="s">
+      <c r="E10" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="47" t="s">
+      <c r="F10" s="51" t="s">
         <v>36</v>
       </c>
       <c r="G10" s="6" t="s">
@@ -4374,10 +5312,10 @@
       </c>
     </row>
     <row r="11" spans="3:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
       <c r="G11" s="6" t="s">
         <v>76</v>
       </c>
@@ -4413,10 +5351,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="56"/>
+      <c r="B1" s="60"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
@@ -4484,11 +5422,11 @@
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
@@ -4505,19 +5443,19 @@
       <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="48" t="s">
+      <c r="E7" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
       <c r="H7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="33" t="s">
+      <c r="I7" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
     </row>
     <row r="8" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
@@ -4530,19 +5468,19 @@
       <c r="D8" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="E8" s="57" t="s">
+      <c r="E8" s="61" t="s">
         <v>79</v>
       </c>
-      <c r="F8" s="58"/>
-      <c r="G8" s="59"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="63"/>
       <c r="H8" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="I8" s="60" t="s">
+      <c r="I8" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="J8" s="61"/>
-      <c r="K8" s="62"/>
+      <c r="J8" s="65"/>
+      <c r="K8" s="66"/>
     </row>
     <row r="9" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
@@ -4555,19 +5493,19 @@
       <c r="D9" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="48" t="s">
+      <c r="E9" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
       <c r="H9" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="I9" s="46" t="s">
+      <c r="I9" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="J9" s="46"/>
-      <c r="K9" s="46"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50"/>
     </row>
     <row r="10" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
@@ -4580,19 +5518,19 @@
       <c r="D10" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="48" t="s">
+      <c r="E10" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
       <c r="H10" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="I10" s="46" t="s">
+      <c r="I10" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="J10" s="46"/>
-      <c r="K10" s="46"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
     </row>
     <row r="11" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
@@ -4605,34 +5543,34 @@
       <c r="D11" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="E11" s="48" t="s">
+      <c r="E11" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
       <c r="H11" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="I11" s="46" t="s">
+      <c r="I11" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="J11" s="46"/>
-      <c r="K11" s="46"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="I11:K11"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="I7:K7"/>
     <mergeCell ref="E8:G8"/>
     <mergeCell ref="I8:K8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="I11:K11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4644,7 +5582,7 @@
   <dimension ref="B5:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4658,135 +5596,136 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="67" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63" t="s">
+      <c r="D5" s="67"/>
+      <c r="E5" s="67" t="s">
         <v>85</v>
       </c>
-      <c r="F5" s="63" t="s">
+      <c r="F5" s="67" t="s">
         <v>86</v>
       </c>
-      <c r="G5" s="63" t="s">
+      <c r="G5" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="H5" s="63" t="s">
+      <c r="H5" s="67" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="63"/>
-    </row>
-    <row r="7" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="63"/>
-      <c r="C7" s="64" t="s">
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
+    </row>
+    <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="67"/>
+      <c r="C7" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="D7" s="64" t="s">
+      <c r="D7" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="63"/>
-    </row>
-    <row r="8" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="65" t="s">
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+    </row>
+    <row r="8" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="C8" s="66">
+      <c r="C8" s="35">
         <v>3</v>
       </c>
-      <c r="D8" s="66">
+      <c r="D8" s="35">
         <v>2</v>
       </c>
-      <c r="E8" s="66">
+      <c r="E8" s="35">
         <v>1</v>
       </c>
-      <c r="F8" s="66">
+      <c r="F8" s="35">
         <f>SUM(C8:E8)</f>
         <v>6</v>
       </c>
-      <c r="G8" s="67">
+      <c r="G8" s="36">
         <f>C8/F8</f>
         <v>0.5</v>
       </c>
-      <c r="H8" s="67">
+      <c r="H8" s="36">
         <f>D8/F8</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B9" s="65" t="s">
+    <row r="9" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="C9" s="66">
+      <c r="C9" s="35">
         <v>3</v>
       </c>
-      <c r="D9" s="66">
+      <c r="D9" s="35">
         <v>3</v>
       </c>
-      <c r="E9" s="66">
+      <c r="E9" s="35">
         <v>0</v>
       </c>
-      <c r="F9" s="66">
+      <c r="F9" s="35">
         <f>SUM(C9:E9)</f>
         <v>6</v>
       </c>
-      <c r="G9" s="67">
+      <c r="G9" s="36">
         <f t="shared" ref="G9:G10" si="0">C9/F9</f>
         <v>0.5</v>
       </c>
-      <c r="H9" s="67">
+      <c r="H9" s="36">
         <f t="shared" ref="H9:H10" si="1">D9/F9</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B10" s="65" t="s">
+    <row r="10" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="66">
+      <c r="C10" s="35">
         <v>0</v>
       </c>
-      <c r="D10" s="66">
+      <c r="D10" s="35">
         <v>4</v>
       </c>
-      <c r="E10" s="66">
+      <c r="E10" s="35">
         <v>0</v>
       </c>
-      <c r="F10" s="66">
+      <c r="F10" s="35">
         <f>SUM(C10:E10)</f>
         <v>4</v>
       </c>
-      <c r="G10" s="67">
+      <c r="G10" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="67">
+      <c r="H10" s="36">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="H5:H7"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="C5:D6"/>
     <mergeCell ref="E5:E7"/>
     <mergeCell ref="F5:F7"/>
     <mergeCell ref="G5:G7"/>
-    <mergeCell ref="H5:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>